<commit_message>
Update latest versions for 4th of July
</commit_message>
<xml_diff>
--- a/logDirectoryOutput.xlsx
+++ b/logDirectoryOutput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simeo\Documents\GitHub\srsRAN-version-compare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e0e0414073b2b33/Documents/GitHub/srsRAN-version-compare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70501300-5851-4C98-80F8-A1915ED27D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{70501300-5851-4C98-80F8-A1915ED27D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3ED18481-6B4A-4020-994F-AD3198AC249B}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="2175" windowWidth="18510" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6120" yWindow="0" windowWidth="19200" windowHeight="11300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logDirectoryOutput" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="75">
   <si>
     <t>Num all files</t>
   </si>
@@ -232,6 +232,21 @@
   </si>
   <si>
     <t>.h (743), .cc (392), .c (354), .txt (130), .dat (39), .cmake (24), .cpp (20),  (12), .example (9), .bin (7), .sh (6), .in (6), .install (5), .md (4), .yml (3), .manpages (3), .service (3), .data (2), .config (1), .postinst (1), .templates (1), .hpp (1), .rst (1)</t>
+  </si>
+  <si>
+    <t>srsRAN-release_22_10</t>
+  </si>
+  <si>
+    <t>srsRAN-release_23_04</t>
+  </si>
+  <si>
+    <t>srsRAN-release_23_04_1</t>
+  </si>
+  <si>
+    <t>.h (743), .cc (392), .c (354), .txt (130), .dat (39), .cmake (23), .cpp (20),  (12), .example (9), .bin (7), .sh (6), .in (6), .install (5), .md (4), .manpages (3), .service (3), .yml (2), .data (2), .config (1), .postinst (1), .templates (1), .hpp (1), .rst (1)</t>
+  </si>
+  <si>
+    <t>.h (757), .cc (399), .c (354), .txt (132), .dat (39), .cpp (24), .cmake (23),  (12), .example (9), .bin (7), .sh (6), .in (6), .install (5), .md (4), .manpages (3), .service (3), .yml (2), .data (2), .config (1), .postinst (1), .templates (1), .hpp (1), .rst (1)</t>
   </si>
 </sst>
 </file>
@@ -1145,29 +1160,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U30"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView topLeftCell="S15" zoomScale="96" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:S27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="1.7109375" style="1" customWidth="1"/>
-    <col min="7" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="1.7109375" style="1" customWidth="1"/>
-    <col min="14" max="16" width="13.7109375" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" style="3" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" style="3" customWidth="1"/>
-    <col min="20" max="20" width="1.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="255.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="5" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="1.7265625" style="1" customWidth="1"/>
+    <col min="7" max="9" width="13.7265625" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.7265625" customWidth="1"/>
+    <col min="12" max="12" width="13.7265625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="1.7265625" style="1" customWidth="1"/>
+    <col min="14" max="16" width="13.7265625" customWidth="1"/>
+    <col min="17" max="17" width="13.7265625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="13.7265625" customWidth="1"/>
+    <col min="19" max="19" width="13.7265625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="1.7265625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="255.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1232,7 +1249,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
@@ -1297,7 +1314,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1362,7 +1379,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -1427,7 +1444,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -1492,7 +1509,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -1557,7 +1574,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1622,7 +1639,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -1687,7 +1704,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -1752,7 +1769,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -1817,7 +1834,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
@@ -1882,7 +1899,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
@@ -1947,7 +1964,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -2012,7 +2029,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -2077,7 +2094,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -2142,7 +2159,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -2207,7 +2224,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -2272,7 +2289,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
@@ -2337,7 +2354,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
@@ -2402,7 +2419,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
@@ -2467,7 +2484,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
@@ -2532,7 +2549,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>46</v>
       </c>
@@ -2597,7 +2614,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>65</v>
       </c>
@@ -2662,7 +2679,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>68</v>
       </c>
@@ -2670,13 +2687,13 @@
         <v>1767</v>
       </c>
       <c r="C24" s="5">
-        <v>57652163</v>
+        <v>58611182</v>
       </c>
       <c r="D24" s="8">
         <v>1558</v>
       </c>
       <c r="E24" s="5">
-        <v>32626111</v>
+        <v>33574041</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>3</v>
@@ -2694,10 +2711,10 @@
         <v>4.9235993208828502E-2</v>
       </c>
       <c r="K24" s="5">
-        <v>2540767</v>
+        <v>2608319</v>
       </c>
       <c r="L24" s="4">
-        <v>4.4070627497532003E-2</v>
+        <v>4.4502071294177201E-2</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>3</v>
@@ -2715,10 +2732,10 @@
         <v>4.7496790757381203E-2</v>
       </c>
       <c r="R24" s="5">
-        <v>2423009</v>
+        <v>2487643</v>
       </c>
       <c r="S24" s="4">
-        <v>7.4265946070005098E-2</v>
+        <v>7.4094238462388204E-2</v>
       </c>
       <c r="T24" s="1" t="s">
         <v>3</v>
@@ -2727,99 +2744,231 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="8">
+        <v>1765</v>
+      </c>
+      <c r="C25" s="5">
+        <v>57659189</v>
+      </c>
+      <c r="D25" s="8">
+        <v>1557</v>
+      </c>
+      <c r="E25" s="5">
+        <v>32632652</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="7">
+        <v>576</v>
+      </c>
+      <c r="H25" s="7">
+        <v>426</v>
+      </c>
+      <c r="I25" s="8">
+        <v>61</v>
+      </c>
+      <c r="J25" s="4">
+        <v>3.4560906515580699E-2</v>
+      </c>
+      <c r="K25" s="5">
+        <v>1439527</v>
+      </c>
+      <c r="L25" s="4">
+        <v>2.49661333252536E-2</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N25" s="7">
+        <v>471</v>
+      </c>
+      <c r="O25" s="7">
+        <v>272</v>
+      </c>
+      <c r="P25" s="8">
+        <v>51</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>3.2755298651252401E-2</v>
+      </c>
+      <c r="R25" s="5">
+        <v>1370728</v>
+      </c>
+      <c r="S25" s="4">
+        <v>4.2004799364758899E-2</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1792</v>
+      </c>
+      <c r="C26" s="5">
+        <v>60362196</v>
+      </c>
+      <c r="D26" s="8">
+        <v>1582</v>
+      </c>
+      <c r="E26" s="5">
+        <v>35332841</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="7">
+        <v>101548</v>
+      </c>
+      <c r="H26" s="7">
+        <v>18273</v>
+      </c>
+      <c r="I26" s="8">
+        <v>1670</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0.93191964285714202</v>
+      </c>
+      <c r="K26" s="5">
+        <v>34724537</v>
+      </c>
+      <c r="L26" s="4">
+        <v>0.57526961080077299</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N26" s="7">
+        <v>101281</v>
+      </c>
+      <c r="O26" s="7">
+        <v>18119</v>
+      </c>
+      <c r="P26" s="8">
+        <v>1532</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>0.96839443742098597</v>
+      </c>
+      <c r="R26" s="5">
+        <v>34378402</v>
+      </c>
+      <c r="S26" s="4">
+        <v>0.97298719907634901</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="8">
+        <v>1792</v>
+      </c>
+      <c r="C27" s="5">
+        <v>60361762</v>
+      </c>
+      <c r="D27" s="8">
+        <v>1582</v>
+      </c>
+      <c r="E27" s="5">
+        <v>35332407</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="7">
+        <v>7</v>
+      </c>
+      <c r="H27" s="7">
         <v>19</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="I27" s="8">
+        <v>2</v>
+      </c>
+      <c r="J27" s="4">
+        <v>1.1160714285714201E-3</v>
+      </c>
+      <c r="K27" s="5">
+        <v>130119</v>
+      </c>
+      <c r="L27" s="4">
+        <v>2.1556527789894499E-3</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N27" s="7">
+        <v>7</v>
+      </c>
+      <c r="O27" s="7">
+        <v>19</v>
+      </c>
+      <c r="P27" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>1.2642225031605501E-3</v>
+      </c>
+      <c r="R27" s="5">
+        <v>130119</v>
+      </c>
+      <c r="S27" s="4">
+        <v>3.6827097570793798E-3</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="G26" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="N26" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="12"/>
-      <c r="R26" s="12"/>
-      <c r="S26" s="12"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="12"/>
-      <c r="R27" s="12"/>
-      <c r="S27" s="12"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="12"/>
-      <c r="S28" s="12"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="11"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
-      <c r="G29" s="11"/>
+      <c r="G29" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
       <c r="K29" s="11"/>
       <c r="L29" s="11"/>
-      <c r="N29" s="12"/>
+      <c r="N29" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="O29" s="12"/>
       <c r="P29" s="12"/>
       <c r="Q29" s="12"/>
       <c r="R29" s="12"/>
       <c r="S29" s="12"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>16</v>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A30" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -2838,11 +2987,74 @@
       <c r="R30" s="12"/>
       <c r="S30" s="12"/>
     </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="12"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="12"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="12"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="G26:L30"/>
-    <mergeCell ref="N26:S30"/>
-    <mergeCell ref="B26:E30"/>
+    <mergeCell ref="G29:L33"/>
+    <mergeCell ref="N29:S33"/>
+    <mergeCell ref="B29:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2850,15 +3062,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BEFFBAC-CDDA-4D6D-95A5-D1E736691CE2}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection sqref="A1:B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -2866,7 +3078,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
@@ -2874,7 +3086,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -2882,7 +3094,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -2890,7 +3102,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -2898,7 +3110,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -2906,7 +3118,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -2914,7 +3126,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -2922,7 +3134,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -2930,7 +3142,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -2938,7 +3150,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
@@ -2946,7 +3158,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
@@ -2954,7 +3166,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -2962,7 +3174,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -2970,7 +3182,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -2978,7 +3190,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -2986,7 +3198,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -2994,7 +3206,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
@@ -3002,7 +3214,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
@@ -3010,7 +3222,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
@@ -3018,7 +3230,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
@@ -3026,7 +3238,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>46</v>
       </c>
@@ -3034,7 +3246,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>65</v>
       </c>
@@ -3042,12 +3254,36 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B24" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>